<commit_message>
Adjust the probe angle; add 644 node model and 253 node with infarct
</commit_message>
<xml_diff>
--- a/src/Refine/Heart_N3_second_138N477P106VM.xlsx
+++ b/src/Refine/Heart_N3_second_138N477P106VM.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5BCB2EE1-6C1E-4050-B2EE-AA42A1686D39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="8_{5BCB2EE1-6C1E-4050-B2EE-AA42A1686D39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{81D8C35F-4C86-4387-A34E-FA655DE1FB5A}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1080" yWindow="1080" windowWidth="21600" windowHeight="12645" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Node_second" sheetId="45" r:id="rId1"/>
@@ -22876,7 +22876,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B535DFB7-3157-441D-AABF-E5C5F2959ADD}">
   <dimension ref="A1:Y478"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A439" workbookViewId="0">
+    <sheetView topLeftCell="A439" workbookViewId="0">
       <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
@@ -59956,8 +59956,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:J9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6:D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -60098,17 +60098,17 @@
         <v>5</v>
       </c>
       <c r="C6">
-        <v>146.14901202656901</v>
+        <v>142</v>
       </c>
       <c r="D6">
-        <v>52.157502287235403</v>
+        <v>45.5</v>
       </c>
       <c r="E6">
         <v>1</v>
       </c>
       <c r="F6">
         <f>SQRT((C7-C8)^2+(D7-D8)^2)</f>
-        <v>9.0000822596236087</v>
+        <v>10.606601717798213</v>
       </c>
       <c r="G6" t="s">
         <v>242</v>
@@ -60133,17 +60133,17 @@
         <v>6</v>
       </c>
       <c r="C7">
-        <v>149.433176079595</v>
+        <v>145</v>
       </c>
       <c r="D7">
-        <v>49.8739614067566</v>
+        <v>45</v>
       </c>
       <c r="E7">
         <v>1</v>
       </c>
       <c r="F7">
         <f>SQRT((C6-C7)^2+(D6-D7)^2)</f>
-        <v>4.0000365598336725</v>
+        <v>3.0413812651491097</v>
       </c>
       <c r="G7" t="s">
         <v>243</v>
@@ -60168,17 +60168,17 @@
         <v>7</v>
       </c>
       <c r="C8">
-        <v>156.822545198901</v>
+        <v>155.5</v>
       </c>
       <c r="D8">
-        <v>44.7359944256795</v>
+        <v>43.5</v>
       </c>
       <c r="E8">
         <v>3</v>
       </c>
       <c r="F8">
         <f t="shared" si="0"/>
-        <v>2.000018279916846</v>
+        <v>2.9616887074775513</v>
       </c>
       <c r="G8" t="s">
         <v>244</v>
@@ -60192,10 +60192,10 @@
         <v>8</v>
       </c>
       <c r="C9">
-        <v>158.46462722541401</v>
+        <v>158.46</v>
       </c>
       <c r="D9">
-        <v>43.594223985440102</v>
+        <v>43.6</v>
       </c>
       <c r="E9">
         <v>3</v>

</xml_diff>